<commit_message>
CV32E40Pv2 Design issues list: updated all remaining opened issues.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_Design_Issue_Summary.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_Design_Issue_Summary.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/OpenHW Group/RTL_freeze_v2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="918" documentId="8_{028D015D-DBC1-468A-A13F-F4A31F1594F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1BECF1D-3AD4-44D6-B65F-098837945EF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08000072-8359-45AE-8740-073B63E91F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{881F227E-37C6-44AA-ACF6-DDA205B93777}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="review" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">review!$F$9:$F$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">review!$F$11:$F$87</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="224">
   <si>
     <t>“Found By” Classification</t>
   </si>
@@ -311,9 +310,6 @@
     <t>some question in rtl,may be it is a bug</t>
   </si>
   <si>
-    <t>still open since 01-2021, no comments, no updates</t>
-  </si>
-  <si>
     <t>Creation Date</t>
   </si>
   <si>
@@ -578,9 +574,6 @@
     <t>Mar 5, 2020</t>
   </si>
   <si>
-    <t>Opened during v1 and not closed at the end of the project</t>
-  </si>
-  <si>
     <t>Not a bug
 Jul 24, 2020</t>
   </si>
@@ -743,6 +736,33 @@
   </si>
   <si>
     <t>Issues found by Lint/Coding Style</t>
+  </si>
+  <si>
+    <t>Waived
+June 4, 2024</t>
+  </si>
+  <si>
+    <t>Waived</t>
+  </si>
+  <si>
+    <t>Not a bug
+June 4, 2024</t>
+  </si>
+  <si>
+    <t>Waived
+June 5, 2024</t>
+  </si>
+  <si>
+    <t>Opened during v1 and not closed at the end of the project
+Just a better good-looking RTL coding style</t>
+  </si>
+  <si>
+    <t>still open since 01-2021, no comments, no updates
+cv32e40p_prefetch_controller doesn't show any incorrect behavior after a lot of non-regressions (and even a lot of test chips).
+It is fully covered in simulation without any waiver, this is either a performance problem not visible in simulation or not a valid assumption at all.</t>
+  </si>
+  <si>
+    <t>Useful issues filtering command for easiest analysis</t>
   </si>
 </sst>
 </file>
@@ -777,7 +797,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,12 +808,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDEE6EF"/>
         <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -853,7 +867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -920,9 +934,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -932,20 +943,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -956,30 +961,21 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -998,6 +994,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1070,6 +1073,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1384,9 +1390,6 @@
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1424,7 +1427,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <f>COUNTIF(review!$H21:$H124, "Inspection")</f>
+        <f>COUNTIF(review!$H24:$H126, "Inspection")</f>
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1436,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <f>COUNTIF(review!$H21:$H124,  "Formal Verification")</f>
+        <f>COUNTIF(review!$H24:$H126,  "Formal Verification")</f>
         <v>18</v>
       </c>
       <c r="D5" s="3"/>
@@ -1446,7 +1449,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="2">
-        <f>COUNTIF(review!$H$21:$H124,  "Lint")</f>
+        <f>COUNTIF(review!$H$24:$H126,  "Lint")</f>
         <v>2</v>
       </c>
       <c r="D6" s="3"/>
@@ -1456,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="2">
-        <f>COUNTIF(review!$H21:$H124,  "Unknown")</f>
+        <f>COUNTIF(review!$H24:$H126,  "Unknown")</f>
         <v>0</v>
       </c>
       <c r="D7" s="3"/>
@@ -1477,7 +1480,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2">
-        <f>COUNTIF(review!$H$21:$H124,  "Simulation (directed)")</f>
+        <f>COUNTIF(review!$H$24:$H126,  "Simulation (directed)")</f>
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1489,7 +1492,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2">
-        <f>COUNTIF(review!$H$21:$H124,  "Simulation (step&amp;compare)")</f>
+        <f>COUNTIF(review!$H$24:$H126,  "Simulation (step&amp;compare)")</f>
         <v>0</v>
       </c>
       <c r="D13" s="3"/>
@@ -1499,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="2">
-        <f>COUNTIF(review!$H$21:$H124,  "Simulation (corev-dv)")</f>
+        <f>COUNTIF(review!$H$24:$H126,  "Simulation (corev-dv)")</f>
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1522,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="2">
-        <f>COUNTIF(review!$D$21:$D$124,  "RTL functional")</f>
+        <f>COUNTIF(review!$D$24:$D$126,  "RTL functional")</f>
         <v>46</v>
       </c>
       <c r="D19" s="3"/>
@@ -1533,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2">
-        <f>COUNTIF(review!$D$21:$D$124,  "RTL coding style")</f>
+        <f>COUNTIF(review!$D$24:$D$126,  "RTL coding style")</f>
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1546,7 +1549,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="2">
-        <f>COUNTIF(review!$D$21:$D$124,  "Non-RTL functional")</f>
+        <f>COUNTIF(review!$D$24:$D$126,  "Non-RTL functional")</f>
         <v>0</v>
       </c>
       <c r="D21" s="3"/>
@@ -1557,7 +1560,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="2">
-        <f>COUNTIF(review!$D$21:$D$124,  "Unreproducible")</f>
+        <f>COUNTIF(review!$D$24:$D$126,  "Unreproducible")</f>
         <v>0</v>
       </c>
       <c r="D22" s="3"/>
@@ -1568,7 +1571,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="2">
-        <f>COUNTIF(review!$D$21:$D$124,  "Invalid")</f>
+        <f>COUNTIF(review!$D$24:$D$126,  "Invalid")</f>
         <v>3</v>
       </c>
       <c r="D23" s="3"/>
@@ -1619,12 +1622,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:N84"/>
+  <dimension ref="B1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
-    <sheetView topLeftCell="A59" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1640,1963 +1642,2000 @@
     <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="17" t="s">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="11"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="18">
+        <v>4</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="18">
+      <c r="E4" s="18">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23">
+        <v>40</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="18">
+        <f>SUM(E3:E5)</f>
+        <v>55</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="18">
+        <f>E6-E7</f>
+        <v>50</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="19"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="18">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="18">
+        <v>35</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="18">
+        <v>46</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="18">
+        <f>F22</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="19"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="18">
+        <v>18</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="9"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="35">
+        <v>20</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="5"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="18">
         <v>4</v>
       </c>
-      <c r="H1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="18">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23">
-        <v>40</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="18">
-        <f>SUM(G1:G3)</f>
-        <v>55</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="18">
-        <f>G4-G5</f>
-        <v>50</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="18">
-        <v>11</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="18">
-        <v>35</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="18">
-        <v>46</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="19"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="19" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17"/>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="19"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E19" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="6">
+        <f>COUNTIF(F24:F78,"=*Resolved*")</f>
+        <v>45</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="N19" s="29"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E20" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="6">
+        <f>COUNTIF(F24:F78,"=*Not a bug*")</f>
+        <v>7</v>
+      </c>
+      <c r="I20" s="34"/>
+      <c r="J20" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="N20" s="29"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E21" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" s="6">
+        <f>COUNTIF(F25:F79,"=*Waived*")</f>
+        <v>3</v>
+      </c>
+      <c r="I21" s="34"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E22" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="6">
+        <f>COUNTIF(F24:F78,"=*Open*")</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="34"/>
+      <c r="J22" s="7">
+        <f>COUNTIF(J24:J78,"=X")</f>
+        <v>8</v>
+      </c>
+      <c r="K22" s="7">
+        <f>COUNTIF(K24:K78,"=X")</f>
+        <v>18</v>
+      </c>
+      <c r="L22" s="7">
+        <f>COUNTIF(L24:L78,"=X")</f>
+        <v>20</v>
+      </c>
+      <c r="M22" s="29">
+        <f>COUNTIF(M24:M78,"=X")</f>
+        <v>4</v>
+      </c>
+      <c r="N22" s="29"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="29"/>
+    </row>
+    <row r="24" spans="2:14" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>169</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="18">
-        <v>4</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="19"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" s="18">
-        <v>18</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="G15" s="24">
-        <v>21</v>
-      </c>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="5:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="F17" s="6">
-        <f>COUNTIF(F21:F75,"=*Resolved*")</f>
-        <v>45</v>
-      </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
-      <c r="N17" s="30"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="38" t="s">
+      <c r="F24" s="27" t="s">
         <v>107</v>
-      </c>
-      <c r="F18" s="6">
-        <f>COUNTIF(F21:F75,"=*Not a bug*")</f>
-        <v>6</v>
-      </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="L18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="M18" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="N18" s="30"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="6">
-        <f>COUNTIF(F21:F75,"=*Open*")</f>
-        <v>4</v>
-      </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="7">
-        <f>COUNTIF(J21:J75,"=X")</f>
-        <v>8</v>
-      </c>
-      <c r="K19" s="7">
-        <f>COUNTIF(K21:K75,"=X")</f>
-        <v>18</v>
-      </c>
-      <c r="L19" s="7">
-        <f>COUNTIF(L21:L75,"=X")</f>
-        <v>20</v>
-      </c>
-      <c r="M19" s="30">
-        <f>COUNTIF(M21:M75,"=X")</f>
-        <v>4</v>
-      </c>
-      <c r="N19" s="30"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="30"/>
-    </row>
-    <row r="21" spans="2:14" ht="25.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
-        <v>169</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-    </row>
-    <row r="22" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
-        <v>170</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-    </row>
-    <row r="23" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <v>174</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L23" s="7"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-    </row>
-    <row r="24" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
-        <v>197</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>76</v>
+        <v>7</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
+      <c r="K24" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="L24" s="7"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+    </row>
+    <row r="25" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
-        <v>252</v>
+        <v>170</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>166</v>
+        <v>73</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>168</v>
+        <v>7</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
+      <c r="K25" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="30"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
     </row>
     <row r="26" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
-        <v>308</v>
+        <v>174</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>169</v>
+        <v>104</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>78</v>
+        <v>7</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
+      <c r="K26" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="L26" s="7"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
     </row>
     <row r="27" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
-        <v>452</v>
+        <v>197</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
     </row>
     <row r="28" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
-        <v>462</v>
+        <v>252</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>115</v>
+        <v>166</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>118</v>
+        <v>5</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>221</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="29"/>
     </row>
     <row r="29" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
-        <v>571</v>
+        <v>308</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="25" t="s">
-        <v>120</v>
+      <c r="I29" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
     </row>
     <row r="30" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
-        <v>598</v>
+        <v>452</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>122</v>
+        <v>111</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>112</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>123</v>
+        <v>5</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K30" s="7"/>
-      <c r="L30" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
     </row>
     <row r="31" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
-        <v>599</v>
+        <v>462</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>209</v>
+        <v>113</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>211</v>
+        <v>114</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="I31" s="25"/>
+        <v>116</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>117</v>
+      </c>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
     </row>
     <row r="32" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>212</v>
+        <v>30</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>214</v>
+        <v>17</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="I32" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
     </row>
     <row r="33" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="I33" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J33" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="K33" s="7"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="N33" s="30"/>
+      <c r="L33" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
     </row>
     <row r="34" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>217</v>
+      <c r="E34" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="I34" s="25"/>
+        <v>208</v>
+      </c>
+      <c r="I34" s="24"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="7"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+    </row>
+    <row r="35" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
-        <v>612</v>
+        <v>600</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="6" t="s">
-        <v>90</v>
+        <v>22</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>212</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="25" t="s">
-        <v>87</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="I35" s="24"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
     </row>
     <row r="36" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
-        <v>629</v>
+        <v>605</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>133</v>
+        <v>124</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="7"/>
       <c r="K36" s="7"/>
-      <c r="L36" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N36" s="29"/>
     </row>
     <row r="37" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
-        <v>650</v>
+        <v>606</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>131</v>
+        <v>213</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>135</v>
+        <v>22</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>215</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I37" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="I37" s="24"/>
+      <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-    </row>
-    <row r="38" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="L37" s="7"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+    </row>
+    <row r="38" spans="2:14" ht="66" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
-        <v>652</v>
+        <v>612</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>137</v>
+      <c r="E38" s="15"/>
+      <c r="F38" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>144</v>
+        <v>5</v>
+      </c>
+      <c r="I38" s="24" t="s">
+        <v>222</v>
       </c>
       <c r="J38" s="7"/>
-      <c r="K38" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L38" s="32"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
     </row>
     <row r="39" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
-        <v>663</v>
+        <v>629</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I39" s="25" t="s">
-        <v>150</v>
+      <c r="I39" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K39" s="7"/>
-      <c r="L39" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L39" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+    </row>
+    <row r="40" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
-        <v>670</v>
+        <v>650</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>90</v>
+        <v>131</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I40" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="J40" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="I40" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="K40" s="7"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="N40" s="30"/>
+      <c r="L40" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
     </row>
     <row r="41" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
-        <v>684</v>
+        <v>652</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="28" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="25" t="s">
-        <v>151</v>
+        <v>7</v>
+      </c>
+      <c r="I41" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-    </row>
-    <row r="42" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="K41" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L41" s="7"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+    </row>
+    <row r="42" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
-        <v>721</v>
+        <v>663</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>137</v>
+        <v>133</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L42" s="32"/>
-    </row>
-    <row r="43" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+    </row>
+    <row r="43" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
-        <v>722</v>
+        <v>670</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F43" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="G43" s="15"/>
-      <c r="H43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L43" s="32"/>
+      <c r="H43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N43" s="29"/>
     </row>
     <row r="44" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B44" s="6">
-        <v>723</v>
+        <v>684</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F44" s="28" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>140</v>
       </c>
       <c r="G44" s="15"/>
-      <c r="H44" s="8" t="s">
+      <c r="H44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+    </row>
+    <row r="45" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
+        <v>721</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" s="15"/>
+      <c r="H45" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L44" s="32"/>
-      <c r="M44" s="30"/>
-      <c r="N44" s="30"/>
-    </row>
-    <row r="45" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
-        <v>724</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="J45" s="7"/>
+      <c r="I45" s="24" t="s">
+        <v>143</v>
+      </c>
       <c r="K45" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L45" s="32"/>
-      <c r="M45" s="30"/>
-      <c r="N45" s="30"/>
-    </row>
-    <row r="46" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>152</v>
+        <v>141</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="J46" s="7"/>
+      <c r="I46" s="24" t="s">
+        <v>143</v>
+      </c>
       <c r="K46" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L46" s="32"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="47" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B47" s="6">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F47" s="28" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="25" t="s">
-        <v>154</v>
+      <c r="I47" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L47" s="32"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L47" s="7"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
     </row>
     <row r="48" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B48" s="6">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F48" s="28" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="25" t="s">
-        <v>153</v>
+      <c r="I48" s="24" t="s">
+        <v>144</v>
       </c>
       <c r="J48" s="7"/>
       <c r="K48" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L48" s="32"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L48" s="7"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
     </row>
     <row r="49" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B49" s="6">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F49" s="28" t="s">
-        <v>109</v>
+        <v>141</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="25" t="s">
-        <v>155</v>
+      <c r="I49" s="24" t="s">
+        <v>144</v>
       </c>
       <c r="J49" s="7"/>
       <c r="K49" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L49" s="32"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L49" s="7"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
     </row>
     <row r="50" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B50" s="6">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F50" s="28" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="25" t="s">
-        <v>156</v>
+      <c r="I50" s="24" t="s">
+        <v>153</v>
       </c>
       <c r="J50" s="7"/>
       <c r="K50" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L50" s="32"/>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L50" s="7"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
     </row>
     <row r="51" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B51" s="6">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F51" s="28" t="s">
-        <v>157</v>
+        <v>141</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="25" t="s">
-        <v>49</v>
+      <c r="I51" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="J51" s="7"/>
       <c r="K51" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L51" s="32"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L51" s="7"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
     </row>
     <row r="52" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B52" s="6">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F52" s="28" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>108</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="25" t="s">
-        <v>144</v>
+      <c r="I52" s="24" t="s">
+        <v>154</v>
       </c>
       <c r="J52" s="7"/>
       <c r="K52" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L52" s="32"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L52" s="7"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
     </row>
     <row r="53" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B53" s="6">
-        <v>741</v>
+        <v>729</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="F53" s="28" t="s">
-        <v>152</v>
+        <v>141</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="25" t="s">
-        <v>145</v>
+      <c r="I53" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="J53" s="7"/>
       <c r="K53" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L53" s="32"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L53" s="7"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
     </row>
     <row r="54" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B54" s="6">
-        <v>742</v>
+        <v>730</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="F54" s="28" t="s">
-        <v>159</v>
+        <v>141</v>
+      </c>
+      <c r="F54" s="27" t="s">
+        <v>156</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="25" t="s">
-        <v>146</v>
+      <c r="I54" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="J54" s="7"/>
       <c r="K54" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L54" s="32"/>
-      <c r="M54" s="30"/>
-      <c r="N54" s="30"/>
+        <v>164</v>
+      </c>
+      <c r="L54" s="7"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
     </row>
     <row r="55" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B55" s="6">
-        <v>756</v>
+        <v>731</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F55" s="29" t="s">
-        <v>161</v>
+        <v>141</v>
+      </c>
+      <c r="F55" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="G55" s="15"/>
-      <c r="H55" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I55" s="26" t="s">
-        <v>45</v>
+      <c r="H55" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="N55" s="30"/>
+      <c r="K55" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L55" s="7"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
     </row>
     <row r="56" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B56" s="6">
-        <v>800</v>
+        <v>741</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>173</v>
+        <v>157</v>
+      </c>
+      <c r="F56" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="G56" s="15"/>
-      <c r="H56" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I56" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J56" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="K56" s="7"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="30"/>
-      <c r="N56" s="30"/>
+      <c r="H56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L56" s="7"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
     </row>
     <row r="57" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B57" s="6">
-        <v>838</v>
+        <v>742</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F57" s="8" t="s">
         <v>157</v>
       </c>
+      <c r="F57" s="27" t="s">
+        <v>158</v>
+      </c>
       <c r="G57" s="15"/>
-      <c r="H57" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I57" s="27" t="s">
-        <v>49</v>
+      <c r="H57" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="24" t="s">
+        <v>145</v>
       </c>
       <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M57" s="30"/>
-      <c r="N57" s="30"/>
+      <c r="K57" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L57" s="7"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
     </row>
     <row r="58" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B58" s="6">
-        <v>840</v>
+        <v>756</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>176</v>
+        <v>159</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>160</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I58" s="27" t="s">
-        <v>49</v>
+      <c r="I58" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
-      <c r="L58" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M58" s="30"/>
-      <c r="N58" s="30"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N58" s="29"/>
     </row>
     <row r="59" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B59" s="6">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I59" s="26" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K59" s="7"/>
-      <c r="L59" s="32"/>
-      <c r="M59" s="30"/>
-      <c r="N59" s="30"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="29"/>
+      <c r="N59" s="29"/>
     </row>
     <row r="60" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B60" s="6">
-        <v>862</v>
+        <v>838</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="6" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="I60" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J60" s="7" t="s">
-        <v>165</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J60" s="7"/>
       <c r="K60" s="7"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="30"/>
-      <c r="N60" s="30"/>
+      <c r="L60" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
     </row>
     <row r="61" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B61" s="6">
-        <v>869</v>
+        <v>840</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="I61" s="26" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
-      <c r="L61" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M61" s="30"/>
-      <c r="N61" s="30"/>
+      <c r="L61" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M61" s="29"/>
+      <c r="N61" s="29"/>
     </row>
     <row r="62" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B62" s="6">
-        <v>870</v>
+        <v>850</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="G62" s="15"/>
       <c r="H62" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I62" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="J62" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="I62" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J62" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="K62" s="7"/>
-      <c r="L62" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M62" s="30"/>
-      <c r="N62" s="30"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="29"/>
+      <c r="N62" s="29"/>
     </row>
     <row r="63" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B63" s="6">
-        <v>876</v>
+        <v>862</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I63" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="J63" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="I63" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>164</v>
+      </c>
       <c r="K63" s="7"/>
-      <c r="L63" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M63" s="30"/>
-      <c r="N63" s="30"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="29"/>
+      <c r="N63" s="29"/>
     </row>
     <row r="64" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B64" s="6">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I64" s="26" t="s">
-        <v>146</v>
+      <c r="I64" s="25" t="s">
+        <v>145</v>
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
-      <c r="L64" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M64" s="30"/>
-      <c r="N64" s="30"/>
+      <c r="L64" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M64" s="29"/>
+      <c r="N64" s="29"/>
     </row>
     <row r="65" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B65" s="6">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G65" s="15"/>
       <c r="H65" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I65" s="26" t="s">
-        <v>146</v>
+      <c r="I65" s="25" t="s">
+        <v>145</v>
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
-      <c r="L65" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M65" s="30"/>
-      <c r="N65" s="30"/>
+      <c r="L65" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M65" s="29"/>
+      <c r="N65" s="29"/>
     </row>
     <row r="66" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B66" s="6">
-        <v>887</v>
+        <v>876</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I66" s="26" t="s">
-        <v>147</v>
+      <c r="I66" s="25" t="s">
+        <v>145</v>
       </c>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
-      <c r="L66" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M66" s="30"/>
-      <c r="N66" s="30"/>
+      <c r="L66" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M66" s="29"/>
+      <c r="N66" s="29"/>
     </row>
     <row r="67" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B67" s="6">
-        <v>888</v>
+        <v>877</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="G67" s="15"/>
-      <c r="H67" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I67" s="26" t="s">
-        <v>147</v>
+      <c r="H67" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" s="25" t="s">
+        <v>145</v>
       </c>
       <c r="J67" s="7"/>
-      <c r="K67" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="L67" s="32"/>
-      <c r="M67" s="30"/>
-      <c r="N67" s="30"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M67" s="29"/>
+      <c r="N67" s="29"/>
     </row>
     <row r="68" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B68" s="6">
-        <v>889</v>
+        <v>880</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I68" s="26" t="s">
-        <v>147</v>
+      <c r="I68" s="25" t="s">
+        <v>145</v>
       </c>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
-      <c r="L68" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M68" s="30"/>
-      <c r="N68" s="30"/>
+      <c r="L68" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
     </row>
     <row r="69" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B69" s="6">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I69" s="26" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="I69" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
-      <c r="L69" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M69" s="30"/>
-      <c r="N69" s="30"/>
+      <c r="L69" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
     </row>
     <row r="70" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B70" s="6">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G70" s="15"/>
-      <c r="H70" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I70" s="26" t="s">
-        <v>147</v>
+      <c r="H70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I70" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M70" s="30"/>
-      <c r="N70" s="30"/>
+      <c r="K70" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="L70" s="7"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
     </row>
     <row r="71" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B71" s="6">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I71" s="26" t="s">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="I71" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="N71" s="30"/>
+      <c r="L71" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M71" s="29"/>
+      <c r="N71" s="29"/>
     </row>
     <row r="72" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B72" s="6">
-        <v>959</v>
+        <v>894</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I72" s="26" t="s">
-        <v>193</v>
+        <v>28</v>
+      </c>
+      <c r="I72" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
-      <c r="L72" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="N72" s="30"/>
+      <c r="L72" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M72" s="29"/>
+      <c r="N72" s="29"/>
     </row>
     <row r="73" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B73" s="6">
-        <v>960</v>
+        <v>896</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I73" s="26" t="s">
-        <v>193</v>
+        <v>29</v>
+      </c>
+      <c r="I73" s="25" t="s">
+        <v>146</v>
       </c>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
-      <c r="L73" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="N73" s="30"/>
+      <c r="L73" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
     </row>
     <row r="74" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B74" s="6">
-        <v>965</v>
+        <v>901</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I74" s="26" t="s">
-        <v>194</v>
+        <v>8</v>
+      </c>
+      <c r="I74" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
-      <c r="L74" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M74" s="30"/>
-      <c r="N74" s="30"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N74" s="29"/>
     </row>
     <row r="75" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B75" s="6">
-        <v>975</v>
+        <v>959</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I75" s="26" t="s">
-        <v>196</v>
+        <v>5</v>
+      </c>
+      <c r="I75" s="25" t="s">
+        <v>191</v>
       </c>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
-      <c r="L75" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="M75" s="30"/>
-      <c r="N75" s="30"/>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F78" s="11"/>
-      <c r="G78" s="16"/>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F79" s="11"/>
-      <c r="G79" s="16"/>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F80" s="11"/>
-      <c r="G80" s="16"/>
+      <c r="L75" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N75" s="29"/>
+    </row>
+    <row r="76" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B76" s="6">
+        <v>960</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G76" s="15"/>
+      <c r="H76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N76" s="29"/>
+    </row>
+    <row r="77" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B77" s="6">
+        <v>965</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G77" s="15"/>
+      <c r="H77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M77" s="29"/>
+      <c r="N77" s="29"/>
+    </row>
+    <row r="78" spans="2:14" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B78" s="6">
+        <v>975</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G78" s="15"/>
+      <c r="H78" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I78" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="M78" s="29"/>
+      <c r="N78" s="29"/>
     </row>
     <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" s="11"/>
@@ -3614,17 +3653,28 @@
       <c r="F84" s="11"/>
       <c r="G84" s="16"/>
     </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F85" s="11"/>
+      <c r="G85" s="16"/>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F86" s="11"/>
+      <c r="G86" s="16"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F1)))</formula>
+  <conditionalFormatting sqref="F19:F1048576 F1:F2 D3:D18">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Waived">
+      <formula>NOT(ISERROR(SEARCH("Waived",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Resolved">
-      <formula>NOT(ISERROR(SEARCH("Resolved",F1)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Not a bug">
-      <formula>NOT(ISERROR(SEARCH("Not a bug",F1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Resolved">
+      <formula>NOT(ISERROR(SEARCH("Resolved",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Not a bug">
+      <formula>NOT(ISERROR(SEARCH("Not a bug",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -3637,6 +3687,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="254d2fc45a10493323dcacd51be5aaf4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="003ab9e0b5c5bed7880e662758cd0922" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -3885,24 +3953,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-    <SharedWithUsers xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3913,6 +3963,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A65D6B25-B4CF-4DD2-B0D1-F3288A654A97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BADFC4B-73B2-4D3F-B591-B9BE4A93E9D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3931,17 +3992,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A65D6B25-B4CF-4DD2-B0D1-F3288A654A97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D76AFA4A-AF05-419D-BE9B-332D578E982D}">
   <ds:schemaRefs>

</xml_diff>